<commit_message>
IND Money Contrac Notes till May 2025
</commit_message>
<xml_diff>
--- a/INDMoney/INDMoney_contract_notes/01_FY_2024-2025/Indmoney-AnnualPnlReport-X7Z0ZG65W7-31-Mar-2025.xlsx
+++ b/INDMoney/INDMoney_contract_notes/01_FY_2024-2025/Indmoney-AnnualPnlReport-X7Z0ZG65W7-31-Mar-2025.xlsx
@@ -566,16 +566,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -768,926 +772,931 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:P39"/>
+  <dimension ref="A2:R39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="14.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="40.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="28.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="8.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="12.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="13.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.01"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>2937195.199238</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>3076218.9</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>-2802.39996899999</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>-0.00095410750015083</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>31211.438759</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.0106262732443173</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>28409.0387900001</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F16" s="2" t="n">
+        <f aca="false">D23*E23</f>
+        <v>197760</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="I20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I20" s="0" t="s">
+      <c r="J20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J20" s="0" t="s">
+      <c r="K20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="0" t="s">
+      <c r="M20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L20" s="0" t="s">
+      <c r="N20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M20" s="0" t="s">
+      <c r="O20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N20" s="0" t="s">
+      <c r="P20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="0" t="s">
+      <c r="Q20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="P20" s="0" t="s">
+      <c r="R20" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <v>87</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>3099.425287</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" s="2" t="n">
         <v>269649.999969</v>
       </c>
-      <c r="G21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="0" t="s">
+      <c r="H21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L21" s="0" t="s">
+      <c r="N21" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O21" s="0" t="s">
+      <c r="O21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P21" s="0" t="s">
+      <c r="R21" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>65.59</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22" s="2" t="n">
         <v>5903.1</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="0" t="s">
+      <c r="H22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L22" s="0" t="s">
+      <c r="N22" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="O22" s="0" t="s">
+      <c r="O22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="P22" s="0" t="s">
+      <c r="R22" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <v>480</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>412</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23" s="2" t="n">
         <v>197760</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="I23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="0" t="s">
+      <c r="J23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="0" t="s">
+      <c r="K23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="0" t="s">
+      <c r="M23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L23" s="0" t="s">
+      <c r="N23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M23" s="0" t="s">
+      <c r="O23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="N23" s="0" t="s">
+      <c r="P23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O23" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" s="0" t="s">
+      <c r="Q23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R23" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <v>1690</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>121.345473</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="F24" s="2" t="n">
         <v>205073.84937</v>
       </c>
-      <c r="G24" s="0" t="s">
+      <c r="H24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="I24" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I24" s="0" t="s">
+      <c r="J24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J24" s="0" t="s">
+      <c r="K24" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="0" t="s">
+      <c r="M24" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="L24" s="0" t="s">
+      <c r="N24" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M24" s="0" t="s">
+      <c r="O24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="N24" s="0" t="s">
+      <c r="P24" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="O24" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" s="0" t="s">
+      <c r="Q24" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R24" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>2010</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" s="2" t="n">
         <v>201000</v>
       </c>
-      <c r="G25" s="0" t="s">
+      <c r="H25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="I25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I25" s="0" t="s">
+      <c r="J25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J25" s="0" t="s">
+      <c r="K25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K25" s="0" t="s">
+      <c r="M25" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L25" s="0" t="s">
+      <c r="N25" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M25" s="0" t="s">
+      <c r="O25" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="N25" s="0" t="s">
+      <c r="P25" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="O25" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="0" t="s">
+      <c r="Q25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R25" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <v>101</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>1997</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" s="2" t="n">
         <v>201697</v>
       </c>
-      <c r="G26" s="0" t="s">
+      <c r="H26" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="I26" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I26" s="0" t="s">
+      <c r="J26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J26" s="0" t="s">
+      <c r="K26" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K26" s="0" t="s">
+      <c r="M26" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L26" s="0" t="s">
+      <c r="N26" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M26" s="0" t="s">
+      <c r="O26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N26" s="0" t="s">
+      <c r="P26" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="O26" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P26" s="0" t="s">
+      <c r="Q26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R26" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <v>31</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>2002.988709</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" s="2" t="n">
         <v>62092.649979</v>
       </c>
-      <c r="G27" s="0" t="s">
+      <c r="H27" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="I27" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I27" s="0" t="s">
+      <c r="J27" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="J27" s="0" t="s">
+      <c r="K27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="K27" s="0" t="s">
+      <c r="M27" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="L27" s="0" t="s">
+      <c r="N27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M27" s="0" t="s">
+      <c r="O27" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="N27" s="0" t="s">
+      <c r="P27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O27" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P27" s="0" t="s">
+      <c r="Q27" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R27" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="1" t="n">
         <v>953</v>
       </c>
-      <c r="F28" s="1" t="n">
+      <c r="F28" s="2" t="n">
         <v>52415</v>
       </c>
-      <c r="G28" s="0" t="s">
+      <c r="H28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="0" t="s">
+      <c r="I28" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="I28" s="0" t="s">
+      <c r="J28" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="J28" s="0" t="s">
+      <c r="K28" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K28" s="0" t="s">
+      <c r="M28" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L28" s="0" t="s">
+      <c r="N28" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M28" s="0" t="s">
+      <c r="O28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="0" t="s">
+      <c r="P28" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="O28" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P28" s="0" t="s">
+      <c r="Q28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R28" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <v>600</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="1" t="n">
         <v>443.5</v>
       </c>
-      <c r="F29" s="1" t="n">
+      <c r="F29" s="2" t="n">
         <v>266100</v>
       </c>
-      <c r="G29" s="0" t="s">
+      <c r="H29" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H29" s="0" t="s">
+      <c r="I29" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I29" s="0" t="s">
+      <c r="J29" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="J29" s="0" t="s">
+      <c r="K29" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K29" s="0" t="s">
+      <c r="M29" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="L29" s="0" t="s">
+      <c r="N29" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="M29" s="0" t="s">
+      <c r="O29" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="N29" s="0" t="s">
+      <c r="P29" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="O29" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P29" s="0" t="s">
+      <c r="Q29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R29" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="D30" s="1" t="n">
         <v>570</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="1" t="n">
         <v>463.2</v>
       </c>
-      <c r="F30" s="1" t="n">
+      <c r="F30" s="2" t="n">
         <v>264024</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="H30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="H30" s="0" t="s">
+      <c r="I30" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I30" s="0" t="s">
+      <c r="J30" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J30" s="0" t="s">
+      <c r="K30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="K30" s="0" t="s">
+      <c r="M30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="L30" s="0" t="s">
+      <c r="N30" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="M30" s="0" t="s">
+      <c r="O30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="N30" s="0" t="s">
+      <c r="P30" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="O30" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P30" s="0" t="s">
+      <c r="Q30" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="D31" s="1" t="n">
         <v>1000</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="1" t="n">
         <v>267.74625</v>
       </c>
-      <c r="F31" s="1" t="n">
+      <c r="F31" s="2" t="n">
         <v>267746.25</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="H31" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="I31" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="I31" s="0" t="s">
+      <c r="J31" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="K31" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K31" s="0" t="s">
+      <c r="M31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="L31" s="0" t="s">
+      <c r="N31" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="M31" s="0" t="s">
+      <c r="O31" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="N31" s="0" t="s">
+      <c r="P31" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="O31" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P31" s="0" t="s">
+      <c r="Q31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R31" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="D32" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="1" t="n">
         <v>1115.223928</v>
       </c>
-      <c r="F32" s="1" t="n">
+      <c r="F32" s="2" t="n">
         <v>156131.34992</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="H32" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="H32" s="0" t="s">
+      <c r="I32" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="I32" s="0" t="s">
+      <c r="J32" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="J32" s="0" t="s">
+      <c r="K32" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="K32" s="0" t="s">
+      <c r="M32" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="L32" s="0" t="s">
+      <c r="N32" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="M32" s="0" t="s">
+      <c r="O32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="N32" s="0" t="s">
+      <c r="P32" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="O32" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P32" s="0" t="s">
+      <c r="Q32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R32" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="D33" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="1" t="n">
         <v>820</v>
       </c>
-      <c r="F33" s="1" t="n">
+      <c r="F33" s="2" t="n">
         <v>50840</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="H33" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="H33" s="0" t="s">
+      <c r="I33" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="I33" s="0" t="s">
+      <c r="J33" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="J33" s="0" t="s">
+      <c r="K33" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="K33" s="0" t="s">
+      <c r="M33" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L33" s="0" t="s">
+      <c r="N33" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="M33" s="0" t="s">
+      <c r="O33" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="N33" s="0" t="s">
+      <c r="P33" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="O33" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P33" s="0" t="s">
+      <c r="Q33" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="D34" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="E34" s="0" t="n">
+      <c r="E34" s="1" t="n">
         <v>868</v>
       </c>
-      <c r="F34" s="1" t="n">
+      <c r="F34" s="2" t="n">
         <v>260400</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="H34" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="H34" s="0" t="s">
+      <c r="I34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I34" s="0" t="s">
+      <c r="J34" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="J34" s="0" t="s">
+      <c r="K34" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="K34" s="0" t="s">
+      <c r="M34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="L34" s="0" t="s">
+      <c r="N34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M34" s="0" t="s">
+      <c r="O34" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="N34" s="0" t="s">
+      <c r="P34" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="O34" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P34" s="0" t="s">
+      <c r="Q34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R34" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="D35" s="1" t="n">
         <v>2660</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="1" t="n">
         <v>100.7</v>
       </c>
-      <c r="F35" s="1" t="n">
+      <c r="F35" s="2" t="n">
         <v>267862</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="H35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H35" s="0" t="s">
+      <c r="I35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="I35" s="0" t="s">
+      <c r="J35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="J35" s="0" t="s">
+      <c r="K35" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="K35" s="0" t="s">
+      <c r="M35" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="L35" s="0" t="s">
+      <c r="N35" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="M35" s="0" t="s">
+      <c r="O35" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="N35" s="0" t="s">
+      <c r="P35" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="O35" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P35" s="0" t="s">
+      <c r="Q35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R35" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="D36" s="1" t="n">
         <v>300</v>
       </c>
-      <c r="E36" s="0" t="n">
+      <c r="E36" s="1" t="n">
         <v>695</v>
       </c>
-      <c r="F36" s="1" t="n">
+      <c r="F36" s="2" t="n">
         <v>208500</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="H36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="0" t="s">
+      <c r="I36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I36" s="0" t="s">
+      <c r="J36" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="J36" s="0" t="s">
+      <c r="K36" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="K36" s="0" t="s">
+      <c r="M36" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="L36" s="0" t="s">
+      <c r="N36" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M36" s="0" t="s">
+      <c r="O36" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="N36" s="0" t="s">
+      <c r="P36" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="O36" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="P36" s="0" t="s">
+      <c r="Q36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R36" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>